<commit_message>
fix distribution and insert check
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_H.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_H.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300162FF-9655-4B30-AA01-2D5BD6681B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5659017-E73A-40D9-A787-6FF03988AEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1549,7 +1549,7 @@
         <v>0.95</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G21" s="3">
         <f>0.9*E21</f>
@@ -1908,7 +1908,7 @@
         <v>0.95</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G32" s="3">
         <f>E32*0.8</f>

</xml_diff>